<commit_message>
Func. Pass, Syn. Error
</commit_message>
<xml_diff>
--- a/brainstorming.xlsx
+++ b/brainstorming.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Verilog_Project\LZ77_Encoder_Decoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF2565F9-F5A2-4376-8DBA-CF72CD5E46F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4F0E4B-48AD-4435-AE56-140ADC1F67A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{7DCA697A-7108-4E3B-8FE8-B9340512EA34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{7DCA697A-7108-4E3B-8FE8-B9340512EA34}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
     <sheet name="工作表2" sheetId="2" r:id="rId2"/>
+    <sheet name="工作表3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -130,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
   <si>
     <t>a</t>
   </si>
@@ -187,12 +188,32 @@
     <t>input ind</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>look ahead buffer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -256,6 +277,14 @@
     </font>
     <font>
       <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -329,7 +358,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -394,6 +423,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -716,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AD934E-2F9C-4E1B-8245-E4C48EB8F69A}">
   <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:R4"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -939,6 +989,13 @@
       <c r="R4" s="3">
         <v>1</v>
       </c>
+      <c r="X4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -1465,8 +1522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5056D9FF-E217-4B3B-A291-6512A52A24BC}">
   <dimension ref="B1:W5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1614,13 +1671,13 @@
       <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="20">
         <v>1</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="19" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="18">
@@ -1748,4 +1805,605 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCCFE333-3291-47AC-8528-F889A36553BC}">
+  <dimension ref="A1:X11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="9" width="3.125" style="2"/>
+    <col min="10" max="10" width="3.125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="3.125" style="24"/>
+    <col min="12" max="19" width="3.125" style="2"/>
+    <col min="20" max="20" width="3.125" style="1"/>
+    <col min="21" max="16384" width="3.125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22">
+        <v>0</v>
+      </c>
+      <c r="C1" s="22">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22">
+        <v>2</v>
+      </c>
+      <c r="E1" s="22">
+        <v>3</v>
+      </c>
+      <c r="F1" s="22">
+        <v>4</v>
+      </c>
+      <c r="G1" s="22">
+        <v>5</v>
+      </c>
+      <c r="H1" s="22">
+        <v>6</v>
+      </c>
+      <c r="I1" s="22">
+        <v>7</v>
+      </c>
+      <c r="J1" s="22">
+        <v>8</v>
+      </c>
+      <c r="K1" s="22">
+        <v>9</v>
+      </c>
+      <c r="L1" s="22">
+        <v>10</v>
+      </c>
+      <c r="M1" s="22">
+        <v>11</v>
+      </c>
+      <c r="N1" s="22">
+        <v>12</v>
+      </c>
+      <c r="O1" s="22">
+        <v>13</v>
+      </c>
+      <c r="P1" s="22">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="22">
+        <v>15</v>
+      </c>
+      <c r="R1" s="22">
+        <v>16</v>
+      </c>
+      <c r="S1" s="22">
+        <v>17</v>
+      </c>
+      <c r="T1" s="22">
+        <v>18</v>
+      </c>
+      <c r="U1" s="22">
+        <v>19</v>
+      </c>
+      <c r="V1" s="22">
+        <v>20</v>
+      </c>
+      <c r="W1" s="22">
+        <v>21</v>
+      </c>
+      <c r="X1" s="22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="20">
+        <v>0</v>
+      </c>
+      <c r="D2" s="20">
+        <v>1</v>
+      </c>
+      <c r="E2" s="18">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="20">
+        <v>1</v>
+      </c>
+      <c r="I2" s="20">
+        <v>9</v>
+      </c>
+      <c r="J2" s="20">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="20">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="19">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="2">
+        <v>5</v>
+      </c>
+      <c r="S2" s="2">
+        <v>8</v>
+      </c>
+      <c r="T2" s="2">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+      <c r="X2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="27">
+        <v>8</v>
+      </c>
+      <c r="C3" s="27">
+        <v>7</v>
+      </c>
+      <c r="D3" s="27">
+        <v>6</v>
+      </c>
+      <c r="E3" s="27">
+        <v>5</v>
+      </c>
+      <c r="F3" s="27">
+        <v>4</v>
+      </c>
+      <c r="G3" s="27">
+        <v>3</v>
+      </c>
+      <c r="H3" s="27">
+        <v>2</v>
+      </c>
+      <c r="I3" s="27">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="K5" s="24">
+        <v>1</v>
+      </c>
+      <c r="L5" s="20">
+        <v>0</v>
+      </c>
+      <c r="M5" s="20">
+        <v>1</v>
+      </c>
+      <c r="N5" s="20">
+        <v>0</v>
+      </c>
+      <c r="O5" s="20">
+        <v>1</v>
+      </c>
+      <c r="P5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>1</v>
+      </c>
+      <c r="R5" s="20">
+        <v>9</v>
+      </c>
+      <c r="S5" s="20"/>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="20">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="K6" s="24">
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <v>1</v>
+      </c>
+      <c r="M6" s="20">
+        <v>0</v>
+      </c>
+      <c r="N6" s="20">
+        <v>1</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>9</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="I7" s="21">
+        <v>1</v>
+      </c>
+      <c r="J7" s="21">
+        <v>0</v>
+      </c>
+      <c r="K7" s="28">
+        <v>1</v>
+      </c>
+      <c r="L7" s="21">
+        <v>0</v>
+      </c>
+      <c r="M7" s="21">
+        <v>1</v>
+      </c>
+      <c r="N7" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="20">
+        <v>1</v>
+      </c>
+      <c r="P7" s="20">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="20">
+        <v>0</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" s="20"/>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
+        <v>3</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="E8" s="21">
+        <v>1</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
+      <c r="G8" s="20">
+        <v>1</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="28">
+        <v>1</v>
+      </c>
+      <c r="L8" s="20">
+        <v>9</v>
+      </c>
+      <c r="M8" s="20">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O8" s="20">
+        <v>0</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T8" s="1">
+        <v>4</v>
+      </c>
+      <c r="U8" s="2">
+        <v>5</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C9" s="20">
+        <v>1</v>
+      </c>
+      <c r="D9" s="21">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>1</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0</v>
+      </c>
+      <c r="G9" s="20">
+        <v>1</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="20">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>9</v>
+      </c>
+      <c r="K9" s="28">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="20">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="20">
+        <v>1</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T9" s="1">
+        <v>5</v>
+      </c>
+      <c r="U9" s="2">
+        <v>6</v>
+      </c>
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21">
+        <v>0</v>
+      </c>
+      <c r="C10" s="20">
+        <v>1</v>
+      </c>
+      <c r="D10" s="20">
+        <v>0</v>
+      </c>
+      <c r="E10" s="20">
+        <v>1</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="20">
+        <v>1</v>
+      </c>
+      <c r="H10" s="20">
+        <v>9</v>
+      </c>
+      <c r="I10" s="20">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="28">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="20">
+        <v>1</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O10" s="2">
+        <v>1</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>5</v>
+      </c>
+      <c r="R10" s="2">
+        <v>8</v>
+      </c>
+      <c r="T10" s="1">
+        <v>6</v>
+      </c>
+      <c r="U10" s="2">
+        <v>8</v>
+      </c>
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B11" s="20">
+        <v>0</v>
+      </c>
+      <c r="C11" s="21">
+        <v>1</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="20">
+        <v>1</v>
+      </c>
+      <c r="F11" s="20">
+        <v>9</v>
+      </c>
+      <c r="G11" s="20">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="20">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="28">
+        <v>1</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="2">
+        <v>5</v>
+      </c>
+      <c r="P11" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T11" s="1">
+        <v>7</v>
+      </c>
+      <c r="U11" s="2">
+        <v>7</v>
+      </c>
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="K4:R4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>